<commit_message>
Added some tests for gameActionTests class
</commit_message>
<xml_diff>
--- a/OurBoardLayout-Test.xlsx
+++ b/OurBoardLayout-Test.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MehmetYilmaz/eclipse-workspace/ClueGame/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Eclipse\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="12825" yWindow="465" windowWidth="12795" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -879,25 +879,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AI50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="22" width="4" customWidth="1"/>
-    <col min="23" max="23" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="35" width="2.83203125" customWidth="1"/>
+    <col min="25" max="35" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>1</v>
       </c>
@@ -1507,7 +1507,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>1</v>
       </c>
@@ -1592,7 +1592,7 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>11</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>1</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>1</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32">
         <v>0</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="X23" s="33"/>
     </row>
-    <row r="24" spans="1:24" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="35"/>
       <c r="B24" s="35"/>
       <c r="C24" s="35"/>
@@ -2717,7 +2717,7 @@
       <c r="W24" s="35"/>
       <c r="X24" s="35"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="34" t="s">
         <v>23</v>
       </c>
@@ -2745,7 +2745,7 @@
       <c r="W25" s="34"/>
       <c r="X25" s="34"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -2771,7 +2771,7 @@
       <c r="W26" s="34"/>
       <c r="X26" s="34"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -2797,7 +2797,7 @@
       <c r="W27" s="34"/>
       <c r="X27" s="34"/>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -2823,7 +2823,7 @@
       <c r="W28" s="34"/>
       <c r="X28" s="34"/>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
@@ -2849,7 +2849,7 @@
       <c r="W29" s="34"/>
       <c r="X29" s="34"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="34"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
@@ -2875,7 +2875,7 @@
       <c r="W30" s="34"/>
       <c r="X30" s="34"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="34"/>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
@@ -2901,7 +2901,7 @@
       <c r="W31" s="34"/>
       <c r="X31" s="34"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
@@ -2927,7 +2927,7 @@
       <c r="W32" s="34"/>
       <c r="X32" s="34"/>
     </row>
-    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -2953,7 +2953,7 @@
       <c r="W33" s="34"/>
       <c r="X33" s="34"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
@@ -2979,7 +2979,7 @@
       <c r="W34" s="34"/>
       <c r="X34" s="34"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
       <c r="C35" s="34"/>
@@ -3005,7 +3005,7 @@
       <c r="W35" s="34"/>
       <c r="X35" s="34"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
@@ -3031,7 +3031,7 @@
       <c r="W36" s="34"/>
       <c r="X36" s="34"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
@@ -3057,7 +3057,7 @@
       <c r="W37" s="34"/>
       <c r="X37" s="34"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
       <c r="C38" s="34"/>
@@ -3083,7 +3083,7 @@
       <c r="W38" s="34"/>
       <c r="X38" s="34"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
@@ -3109,7 +3109,7 @@
       <c r="W39" s="34"/>
       <c r="X39" s="34"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
@@ -3135,7 +3135,7 @@
       <c r="W40" s="34"/>
       <c r="X40" s="34"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
       <c r="C41" s="34"/>
@@ -3161,7 +3161,7 @@
       <c r="W41" s="34"/>
       <c r="X41" s="34"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
       <c r="C42" s="34"/>
@@ -3187,7 +3187,7 @@
       <c r="W42" s="34"/>
       <c r="X42" s="34"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
       <c r="C43" s="34"/>
@@ -3213,7 +3213,7 @@
       <c r="W43" s="34"/>
       <c r="X43" s="34"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
       <c r="C44" s="34"/>
@@ -3239,7 +3239,7 @@
       <c r="W44" s="34"/>
       <c r="X44" s="34"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
       <c r="C45" s="34"/>
@@ -3265,7 +3265,7 @@
       <c r="W45" s="34"/>
       <c r="X45" s="34"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
       <c r="C46" s="34"/>
@@ -3291,7 +3291,7 @@
       <c r="W46" s="34"/>
       <c r="X46" s="34"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="34"/>
       <c r="B47" s="34"/>
       <c r="C47" s="34"/>
@@ -3317,7 +3317,7 @@
       <c r="W47" s="34"/>
       <c r="X47" s="34"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
       <c r="C48" s="34"/>
@@ -3343,7 +3343,7 @@
       <c r="W48" s="34"/>
       <c r="X48" s="34"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="34"/>
       <c r="B49" s="34"/>
       <c r="C49" s="34"/>
@@ -3369,7 +3369,7 @@
       <c r="W49" s="34"/>
       <c r="X49" s="34"/>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34"/>
       <c r="B50" s="34"/>
       <c r="C50" s="34"/>

</xml_diff>

<commit_message>
Added testSuggestions in gameActionTests
</commit_message>
<xml_diff>
--- a/OurBoardLayout-Test.xlsx
+++ b/OurBoardLayout-Test.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Eclipse\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reed\Document\College Documents\2019-2020\Software Engineering\Eclipse Workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714D5B71-8773-4D7B-8E27-7AB94C6F7930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12825" yWindow="465" windowWidth="12795" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -322,7 +329,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -878,26 +885,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AI50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="22" width="4" customWidth="1"/>
-    <col min="23" max="23" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="35" width="2.85546875" customWidth="1"/>
+    <col min="23" max="23" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="35" width="2.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -972,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>1</v>
       </c>
@@ -1507,7 +1514,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>1</v>
       </c>
@@ -1592,7 +1599,7 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
@@ -1677,7 +1684,7 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
@@ -1762,7 +1769,7 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
@@ -1847,7 +1854,7 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
@@ -1922,7 +1929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
@@ -2072,7 +2079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
@@ -2147,7 +2154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>11</v>
       </c>
@@ -2222,7 +2229,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
@@ -2297,7 +2304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>1</v>
       </c>
@@ -2372,7 +2379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>1</v>
       </c>
@@ -2447,7 +2454,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
@@ -2522,7 +2529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
@@ -2597,7 +2604,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32">
         <v>0</v>
       </c>
@@ -2691,7 +2698,7 @@
       </c>
       <c r="X23" s="33"/>
     </row>
-    <row r="24" spans="1:24" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="35"/>
       <c r="C24" s="35"/>
@@ -2717,7 +2724,7 @@
       <c r="W24" s="35"/>
       <c r="X24" s="35"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>23</v>
       </c>
@@ -2745,7 +2752,7 @@
       <c r="W25" s="34"/>
       <c r="X25" s="34"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -2771,7 +2778,7 @@
       <c r="W26" s="34"/>
       <c r="X26" s="34"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -2797,7 +2804,7 @@
       <c r="W27" s="34"/>
       <c r="X27" s="34"/>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -2823,7 +2830,7 @@
       <c r="W28" s="34"/>
       <c r="X28" s="34"/>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
@@ -2849,7 +2856,7 @@
       <c r="W29" s="34"/>
       <c r="X29" s="34"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
@@ -2875,7 +2882,7 @@
       <c r="W30" s="34"/>
       <c r="X30" s="34"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
@@ -2901,7 +2908,7 @@
       <c r="W31" s="34"/>
       <c r="X31" s="34"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
@@ -2927,7 +2934,7 @@
       <c r="W32" s="34"/>
       <c r="X32" s="34"/>
     </row>
-    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -2953,7 +2960,7 @@
       <c r="W33" s="34"/>
       <c r="X33" s="34"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
@@ -2979,7 +2986,7 @@
       <c r="W34" s="34"/>
       <c r="X34" s="34"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
       <c r="C35" s="34"/>
@@ -3005,7 +3012,7 @@
       <c r="W35" s="34"/>
       <c r="X35" s="34"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
@@ -3031,7 +3038,7 @@
       <c r="W36" s="34"/>
       <c r="X36" s="34"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
@@ -3057,7 +3064,7 @@
       <c r="W37" s="34"/>
       <c r="X37" s="34"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
       <c r="C38" s="34"/>
@@ -3083,7 +3090,7 @@
       <c r="W38" s="34"/>
       <c r="X38" s="34"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
@@ -3109,7 +3116,7 @@
       <c r="W39" s="34"/>
       <c r="X39" s="34"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
@@ -3135,7 +3142,7 @@
       <c r="W40" s="34"/>
       <c r="X40" s="34"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
       <c r="B41" s="34"/>
       <c r="C41" s="34"/>
@@ -3161,7 +3168,7 @@
       <c r="W41" s="34"/>
       <c r="X41" s="34"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
       <c r="B42" s="34"/>
       <c r="C42" s="34"/>
@@ -3187,7 +3194,7 @@
       <c r="W42" s="34"/>
       <c r="X42" s="34"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34"/>
       <c r="B43" s="34"/>
       <c r="C43" s="34"/>
@@ -3213,7 +3220,7 @@
       <c r="W43" s="34"/>
       <c r="X43" s="34"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
       <c r="C44" s="34"/>
@@ -3239,7 +3246,7 @@
       <c r="W44" s="34"/>
       <c r="X44" s="34"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
       <c r="C45" s="34"/>
@@ -3265,7 +3272,7 @@
       <c r="W45" s="34"/>
       <c r="X45" s="34"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34"/>
       <c r="B46" s="34"/>
       <c r="C46" s="34"/>
@@ -3291,7 +3298,7 @@
       <c r="W46" s="34"/>
       <c r="X46" s="34"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="34"/>
       <c r="B47" s="34"/>
       <c r="C47" s="34"/>
@@ -3317,7 +3324,7 @@
       <c r="W47" s="34"/>
       <c r="X47" s="34"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="34"/>
       <c r="B48" s="34"/>
       <c r="C48" s="34"/>
@@ -3343,7 +3350,7 @@
       <c r="W48" s="34"/>
       <c r="X48" s="34"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34"/>
       <c r="B49" s="34"/>
       <c r="C49" s="34"/>
@@ -3369,7 +3376,7 @@
       <c r="W49" s="34"/>
       <c r="X49" s="34"/>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34"/>
       <c r="B50" s="34"/>
       <c r="C50" s="34"/>

</xml_diff>